<commit_message>
Bom List New  V1.3
</commit_message>
<xml_diff>
--- a/List linh kien/BOM list.xlsx
+++ b/List linh kien/BOM list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manht\Desktop\DATN\List linh kien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69201888-C61B-47FB-A2EB-FEE9D0FC7B09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81941225-CDD2-4F22-90FA-E1B68718B11F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7C70D7B4-A921-411A-82F4-630251E4D39B}"/>
   </bookViews>
@@ -2088,8 +2088,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3110,7 +3110,7 @@
         <f t="shared" si="0"/>
         <v>5000</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="9" t="s">
         <v>501</v>
       </c>
       <c r="K23" t="s">
@@ -5839,8 +5839,9 @@
     <hyperlink ref="J27" r:id="rId16" xr:uid="{213C53D5-5F44-46CD-B762-E71EBABFACE5}"/>
     <hyperlink ref="J63" r:id="rId17" xr:uid="{0819FF95-2112-4C6F-BDFF-61F809671C26}"/>
     <hyperlink ref="J86" r:id="rId18" xr:uid="{231D7A20-B402-4E54-A7FF-72F0FFA9CE48}"/>
+    <hyperlink ref="J23" r:id="rId19" xr:uid="{596381A0-E97A-41B8-A13E-84507AEEBF15}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>